<commit_message>
Code and data corrections to calculate dissolved gas concentration. Still need to integrate into mergePredictors.R and data paper.
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/ADA/CH4_003_Lake O' the Pines/dataSheets/surgeData003.xlsx
+++ b/SuRGE_Sharepoint/data/ADA/CH4_003_Lake O' the Pines/dataSheets/surgeData003.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/data/ADA/CH4_003_Lake O' the Pines/dataSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/SuRGE/SuRGE_Sharepoint/data/ADA/CH4_003_Lake O' the Pines/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1573" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{709E4EC3-22F9-452E-8BE4-EA127E7C444B}"/>
+  <xr:revisionPtr revIDLastSave="1574" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59CD2FFB-1214-407C-A698-C09A3C7AF374}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="34560" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -767,7 +767,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1434,9 +1434,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1474,7 +1474,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1580,7 +1580,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1722,7 +1722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1733,88 +1733,88 @@
   <dimension ref="A1:BZ27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="BT17" sqref="BT17:BV17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="6" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="15" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="10" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="72" max="74" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="74" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="17" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="BY1" s="32"/>
       <c r="BZ1" s="32"/>
     </row>
-    <row r="2" spans="1:78">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:78">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>84</v>
       </c>
@@ -2236,15 +2236,6 @@
       <c r="BE3">
         <v>13.9</v>
       </c>
-      <c r="BT3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>92</v>
-      </c>
       <c r="BW3">
         <v>2.0499999999999998</v>
       </c>
@@ -2258,7 +2249,7 @@
         <v>0.84550925925925924</v>
       </c>
     </row>
-    <row r="4" spans="1:78">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>84</v>
       </c>
@@ -2350,7 +2341,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="5" spans="1:78">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>84</v>
       </c>
@@ -2442,7 +2433,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="6" spans="1:78">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>84</v>
       </c>
@@ -2543,7 +2534,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="7" spans="1:78">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>84</v>
       </c>
@@ -2638,7 +2629,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="8" spans="1:78">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>84</v>
       </c>
@@ -2736,7 +2727,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="9" spans="1:78">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>84</v>
       </c>
@@ -2810,7 +2801,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:78">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>84</v>
       </c>
@@ -2902,7 +2893,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="11" spans="1:78">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>84</v>
       </c>
@@ -2942,7 +2933,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="12" spans="1:78">
+    <row r="12" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>84</v>
       </c>
@@ -3034,7 +3025,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="13" spans="1:78">
+    <row r="13" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>84</v>
       </c>
@@ -3126,7 +3117,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="14" spans="1:78">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>84</v>
       </c>
@@ -3221,7 +3212,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="15" spans="1:78">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>84</v>
       </c>
@@ -3313,7 +3304,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="16" spans="1:78">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>84</v>
       </c>
@@ -3405,7 +3396,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="17" spans="1:57">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>84</v>
       </c>
@@ -3505,8 +3496,17 @@
       <c r="BE17">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:57">
+      <c r="BT17" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU17" t="s">
+        <v>91</v>
+      </c>
+      <c r="BV17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>84</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="19" spans="1:57">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>84</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:57">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>84</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:57">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>84</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="22" spans="1:57">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>84</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:57">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>84</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:57">
+    <row r="24" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>84</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:57">
+    <row r="25" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>84</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:57">
+    <row r="26" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>84</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:57">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>84</v>
       </c>
@@ -4014,14 +4014,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="116.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="116.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="72">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -4804,17 +4804,17 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="25"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="25"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>5</v>
       </c>
@@ -4830,7 +4830,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
@@ -4864,7 +4864,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>84</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>84</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>84</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>84</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>84</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>84</v>
       </c>
@@ -5055,14 +5055,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>212</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>213</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>214</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>215</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>216</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>217</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>218</v>
       </c>
@@ -5646,6 +5646,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
@@ -5687,32 +5701,55 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C85FBCBD-0D3B-418B-B4E0-D65FBB5D508E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C85FBCBD-0D3B-418B-B4E0-D65FBB5D508E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="8b03727f-4454-4722-b3e6-018d8dcaf2fd"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>